<commit_message>
Debi - Check Call Monitoring Changes
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\udminsure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F0FF93-946E-4D4B-94C1-11B754109D4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042D18FF-8719-4767-AAC0-F0C3832997E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="98">
   <si>
     <t>BANKING DETAILS</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>Total Upgrade Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was debi-check explained correctly? </t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -710,6 +713,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -896,6 +919,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -903,12 +932,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1249,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC331D33-4154-4CDD-B7F8-E59F04140001}">
-  <dimension ref="A1:CF9"/>
+  <dimension ref="A1:CG9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="CD9" sqref="CD9"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,23 +1296,23 @@
     <col min="22" max="22" width="18.5703125" customWidth="1"/>
     <col min="23" max="23" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="48" width="15.42578125" customWidth="1"/>
-    <col min="49" max="49" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="47.140625" customWidth="1"/>
-    <col min="52" max="52" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="31.42578125" customWidth="1"/>
-    <col min="54" max="54" width="12.7109375" customWidth="1"/>
-    <col min="55" max="55" width="28" customWidth="1"/>
-    <col min="56" max="56" width="18.7109375" customWidth="1"/>
-    <col min="57" max="57" width="13.5703125" customWidth="1"/>
-    <col min="58" max="58" width="13" customWidth="1"/>
-    <col min="59" max="59" width="14" customWidth="1"/>
-    <col min="60" max="60" width="12.28515625" customWidth="1"/>
-    <col min="61" max="61" width="13.140625" customWidth="1"/>
-    <col min="74" max="84" width="9.140625" style="48"/>
+    <col min="25" max="49" width="15.42578125" customWidth="1"/>
+    <col min="50" max="50" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="47.140625" customWidth="1"/>
+    <col min="53" max="53" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="31.42578125" customWidth="1"/>
+    <col min="55" max="55" width="12.7109375" customWidth="1"/>
+    <col min="56" max="56" width="28" customWidth="1"/>
+    <col min="57" max="57" width="18.7109375" customWidth="1"/>
+    <col min="58" max="58" width="13.5703125" customWidth="1"/>
+    <col min="59" max="59" width="13" customWidth="1"/>
+    <col min="60" max="60" width="14" customWidth="1"/>
+    <col min="61" max="61" width="12.28515625" customWidth="1"/>
+    <col min="62" max="62" width="13.140625" customWidth="1"/>
+    <col min="75" max="85" width="9.140625" style="48"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:85" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="51" t="s">
         <v>52</v>
       </c>
@@ -1375,9 +1398,10 @@
       <c r="CC1" s="52"/>
       <c r="CD1" s="52"/>
       <c r="CE1" s="52"/>
-    </row>
-    <row r="2" spans="1:84" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="CF1" s="52"/>
+    </row>
+    <row r="2" spans="1:85" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
         <v>37</v>
       </c>
@@ -1435,9 +1459,10 @@
       <c r="BA3" s="56"/>
       <c r="BB3" s="56"/>
       <c r="BC3" s="56"/>
-    </row>
-    <row r="4" spans="1:84" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="BD3" s="56"/>
+    </row>
+    <row r="4" spans="1:85" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -1449,8 +1474,8 @@
       <c r="E5" s="42"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:84" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:84" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:85" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:85" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="57" t="s">
         <v>35</v>
       </c>
@@ -1485,72 +1510,73 @@
       <c r="AB7" s="61"/>
       <c r="AC7" s="61"/>
       <c r="AD7" s="61"/>
-      <c r="AE7" s="62"/>
-      <c r="AF7" s="63" t="s">
+      <c r="AE7" s="61"/>
+      <c r="AF7" s="62"/>
+      <c r="AG7" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="AG7" s="64"/>
       <c r="AH7" s="64"/>
       <c r="AI7" s="64"/>
       <c r="AJ7" s="64"/>
       <c r="AK7" s="64"/>
       <c r="AL7" s="64"/>
       <c r="AM7" s="64"/>
-      <c r="AN7" s="65"/>
-      <c r="AO7" s="66" t="s">
+      <c r="AN7" s="64"/>
+      <c r="AO7" s="65"/>
+      <c r="AP7" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="AP7" s="67"/>
       <c r="AQ7" s="67"/>
       <c r="AR7" s="67"/>
       <c r="AS7" s="67"/>
       <c r="AT7" s="67"/>
       <c r="AU7" s="67"/>
-      <c r="AV7" s="68"/>
-      <c r="AW7" s="57" t="s">
+      <c r="AV7" s="67"/>
+      <c r="AW7" s="68"/>
+      <c r="AX7" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="AX7" s="58"/>
       <c r="AY7" s="58"/>
       <c r="AZ7" s="58"/>
       <c r="BA7" s="58"/>
       <c r="BB7" s="58"/>
       <c r="BC7" s="58"/>
-      <c r="BD7" s="53" t="s">
+      <c r="BD7" s="58"/>
+      <c r="BE7" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="BE7" s="54"/>
       <c r="BF7" s="54"/>
       <c r="BG7" s="54"/>
       <c r="BH7" s="54"/>
-      <c r="BI7" s="55"/>
-      <c r="BJ7" s="74" t="s">
+      <c r="BI7" s="54"/>
+      <c r="BJ7" s="55"/>
+      <c r="BK7" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="BK7" s="75"/>
-      <c r="BL7" s="75"/>
-      <c r="BM7" s="75"/>
-      <c r="BN7" s="75"/>
-      <c r="BO7" s="75"/>
-      <c r="BP7" s="75"/>
-      <c r="BQ7" s="75"/>
-      <c r="BR7" s="75"/>
-      <c r="BS7" s="75"/>
-      <c r="BT7" s="75"/>
-      <c r="BU7" s="75"/>
-      <c r="BV7" s="75"/>
-      <c r="BW7" s="75"/>
-      <c r="BX7" s="75"/>
-      <c r="BY7" s="75"/>
-      <c r="BZ7" s="75"/>
-      <c r="CA7" s="75"/>
-      <c r="CB7" s="75"/>
-      <c r="CC7" s="75"/>
-      <c r="CD7" s="75"/>
-      <c r="CE7" s="75"/>
-      <c r="CF7" s="75"/>
-    </row>
-    <row r="8" spans="1:84" s="2" customFormat="1" ht="57.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL7" s="72"/>
+      <c r="BM7" s="72"/>
+      <c r="BN7" s="72"/>
+      <c r="BO7" s="72"/>
+      <c r="BP7" s="72"/>
+      <c r="BQ7" s="72"/>
+      <c r="BR7" s="72"/>
+      <c r="BS7" s="72"/>
+      <c r="BT7" s="72"/>
+      <c r="BU7" s="72"/>
+      <c r="BV7" s="72"/>
+      <c r="BW7" s="72"/>
+      <c r="BX7" s="72"/>
+      <c r="BY7" s="72"/>
+      <c r="BZ7" s="72"/>
+      <c r="CA7" s="72"/>
+      <c r="CB7" s="72"/>
+      <c r="CC7" s="72"/>
+      <c r="CD7" s="72"/>
+      <c r="CE7" s="72"/>
+      <c r="CF7" s="72"/>
+      <c r="CG7" s="72"/>
+    </row>
+    <row r="8" spans="1:85" s="2" customFormat="1" ht="57.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1639,172 +1665,175 @@
         <v>33</v>
       </c>
       <c r="AD8" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="AE8" s="33" t="s">
+      <c r="AF8" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="AF8" s="21" t="s">
+      <c r="AG8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="AG8" s="10" t="s">
+      <c r="AH8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AH8" s="10" t="s">
+      <c r="AI8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AI8" s="10" t="s">
+      <c r="AJ8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AJ8" s="10" t="s">
+      <c r="AK8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AK8" s="10" t="s">
+      <c r="AL8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AL8" s="10" t="s">
+      <c r="AM8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AM8" s="22" t="s">
+      <c r="AN8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AN8" s="22" t="s">
+      <c r="AO8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="AO8" s="18" t="s">
+      <c r="AP8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="AP8" s="11" t="s">
+      <c r="AQ8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="AQ8" s="11" t="s">
+      <c r="AR8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="AR8" s="11" t="s">
+      <c r="AS8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AS8" s="11" t="s">
+      <c r="AT8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AT8" s="11" t="s">
+      <c r="AU8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AU8" s="11" t="s">
+      <c r="AV8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AV8" s="19" t="s">
+      <c r="AW8" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="AW8" s="34" t="s">
+      <c r="AX8" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="AX8" s="37" t="s">
+      <c r="AY8" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="AY8" s="35" t="s">
+      <c r="AZ8" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="AZ8" s="35" t="s">
+      <c r="BA8" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="BA8" s="36" t="s">
+      <c r="BB8" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="BB8" s="36" t="s">
+      <c r="BC8" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="BC8" s="15" t="s">
+      <c r="BD8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="BD8" s="44" t="s">
+      <c r="BE8" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="BE8" s="44" t="s">
+      <c r="BF8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="BF8" s="44" t="s">
+      <c r="BG8" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="BG8" s="44" t="s">
+      <c r="BH8" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="BH8" s="44" t="s">
+      <c r="BI8" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="BI8" s="44" t="s">
+      <c r="BJ8" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="BJ8" s="46" t="s">
+      <c r="BK8" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="BK8" s="46" t="s">
+      <c r="BL8" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="BL8" s="46" t="s">
+      <c r="BM8" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="BM8" s="46" t="s">
+      <c r="BN8" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="BN8" s="46" t="s">
+      <c r="BO8" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="BO8" s="46" t="s">
+      <c r="BP8" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="BP8" s="45" t="s">
+      <c r="BQ8" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="BQ8" s="45" t="s">
+      <c r="BR8" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="BR8" s="45" t="s">
+      <c r="BS8" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="BS8" s="45" t="s">
+      <c r="BT8" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="BT8" s="45" t="s">
+      <c r="BU8" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="BU8" s="45" t="s">
+      <c r="BV8" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="BV8" s="49" t="s">
+      <c r="BW8" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="BW8" s="49" t="s">
+      <c r="BX8" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="BX8" s="49" t="s">
+      <c r="BY8" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="BY8" s="49" t="s">
+      <c r="BZ8" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="BZ8" s="49" t="s">
+      <c r="CA8" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="CA8" s="49" t="s">
+      <c r="CB8" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="CB8" s="49" t="s">
+      <c r="CC8" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="CC8" s="49" t="s">
+      <c r="CD8" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="CD8" s="49" t="s">
+      <c r="CE8" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="CE8" s="49" t="s">
+      <c r="CF8" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="CF8" s="49" t="s">
+      <c r="CG8" s="49" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:84" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -1872,11 +1901,11 @@
         <v>39</v>
       </c>
       <c r="AE9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF9" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="AF9" s="23" t="s">
-        <v>39</v>
-      </c>
       <c r="AG9" s="23" t="s">
         <v>39</v>
       </c>
@@ -1925,14 +1954,16 @@
       <c r="AV9" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="AW9" s="4"/>
+      <c r="AW9" s="23" t="s">
+        <v>39</v>
+      </c>
       <c r="AX9" s="4"/>
       <c r="AY9" s="4"/>
-      <c r="AZ9" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="BA9" s="23"/>
-      <c r="BB9" s="4"/>
+      <c r="AZ9" s="4"/>
+      <c r="BA9" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB9" s="23"/>
       <c r="BC9" s="4"/>
       <c r="BD9" s="4"/>
       <c r="BE9" s="4"/>
@@ -1940,7 +1971,7 @@
       <c r="BG9" s="4"/>
       <c r="BH9" s="4"/>
       <c r="BI9" s="4"/>
-      <c r="BJ9" s="47"/>
+      <c r="BJ9" s="4"/>
       <c r="BK9" s="47"/>
       <c r="BL9" s="47"/>
       <c r="BM9" s="47"/>
@@ -1952,7 +1983,7 @@
       <c r="BS9" s="47"/>
       <c r="BT9" s="47"/>
       <c r="BU9" s="47"/>
-      <c r="BV9" s="50"/>
+      <c r="BV9" s="47"/>
       <c r="BW9" s="50"/>
       <c r="BX9" s="50"/>
       <c r="BY9" s="50"/>
@@ -1963,19 +1994,20 @@
       <c r="CD9" s="50"/>
       <c r="CE9" s="50"/>
       <c r="CF9" s="50"/>
+      <c r="CG9" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A1:CE1"/>
-    <mergeCell ref="BD7:BI7"/>
-    <mergeCell ref="A3:BC3"/>
+    <mergeCell ref="A1:CF1"/>
+    <mergeCell ref="BE7:BJ7"/>
+    <mergeCell ref="A3:BD3"/>
     <mergeCell ref="A7:X7"/>
-    <mergeCell ref="Y7:AE7"/>
-    <mergeCell ref="AF7:AN7"/>
-    <mergeCell ref="AO7:AV7"/>
-    <mergeCell ref="AW7:BC7"/>
+    <mergeCell ref="Y7:AF7"/>
+    <mergeCell ref="AG7:AO7"/>
+    <mergeCell ref="AP7:AW7"/>
+    <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="BJ7:CF7"/>
+    <mergeCell ref="BK7:CG7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2015,52 +2047,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="72"/>
-      <c r="AH1" s="72"/>
-      <c r="AI1" s="72"/>
-      <c r="AJ1" s="72"/>
-      <c r="AK1" s="72"/>
-      <c r="AL1" s="72"/>
-      <c r="AM1" s="72"/>
-      <c r="AN1" s="72"/>
-      <c r="AO1" s="72"/>
-      <c r="AP1" s="72"/>
-      <c r="AQ1" s="72"/>
-      <c r="AR1" s="73"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="74"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
+      <c r="X1" s="74"/>
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="74"/>
+      <c r="AA1" s="74"/>
+      <c r="AB1" s="74"/>
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="74"/>
+      <c r="AF1" s="74"/>
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="74"/>
+      <c r="AI1" s="74"/>
+      <c r="AJ1" s="74"/>
+      <c r="AK1" s="74"/>
+      <c r="AL1" s="74"/>
+      <c r="AM1" s="74"/>
+      <c r="AN1" s="74"/>
+      <c r="AO1" s="74"/>
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="74"/>
+      <c r="AR1" s="75"/>
     </row>
     <row r="2" spans="1:44" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added the last two columns on the Call Monitoring Report Template
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaneB\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042D18FF-8719-4767-AAC0-F0C3832997E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA939C5-8B0C-433D-8E54-C7A671FDD7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CallMonitoringReport" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="99">
   <si>
     <t>BANKING DETAILS</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t xml:space="preserve">Was debi-check explained correctly? </t>
+  </si>
+  <si>
+    <t>Debi-Check Mandate Status</t>
   </si>
 </sst>
 </file>
@@ -329,7 +332,7 @@
     <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,8 +386,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +473,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -736,10 +752,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -859,6 +876,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -919,12 +946,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -935,7 +956,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1272,311 +1294,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC331D33-4154-4CDD-B7F8-E59F04140001}">
-  <dimension ref="A1:CG9"/>
+  <dimension ref="A1:CH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView topLeftCell="BP1" workbookViewId="0">
+      <selection activeCell="BQ8" sqref="BQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="10" width="32.85546875" customWidth="1"/>
-    <col min="11" max="14" width="28" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.7109375" customWidth="1"/>
-    <col min="21" max="21" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="48.140625" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" customWidth="1"/>
+    <col min="9" max="9" width="45.7109375" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" customWidth="1"/>
+    <col min="11" max="11" width="34.140625" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" customWidth="1"/>
+    <col min="13" max="13" width="34.85546875" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" customWidth="1"/>
+    <col min="21" max="21" width="40.85546875" customWidth="1"/>
     <col min="22" max="22" width="18.5703125" customWidth="1"/>
-    <col min="23" max="23" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="49" width="15.42578125" customWidth="1"/>
-    <col min="50" max="50" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="47.140625" customWidth="1"/>
+    <col min="23" max="23" width="17.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.7109375" customWidth="1"/>
+    <col min="25" max="31" width="15.42578125" customWidth="1"/>
+    <col min="32" max="32" width="24.140625" customWidth="1"/>
+    <col min="33" max="49" width="15.42578125" customWidth="1"/>
+    <col min="50" max="50" width="22.140625" customWidth="1"/>
+    <col min="51" max="51" width="53" customWidth="1"/>
+    <col min="52" max="52" width="47.140625" customWidth="1"/>
     <col min="53" max="53" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="31.42578125" customWidth="1"/>
     <col min="55" max="55" width="12.7109375" customWidth="1"/>
     <col min="56" max="56" width="28" customWidth="1"/>
-    <col min="57" max="57" width="18.7109375" customWidth="1"/>
-    <col min="58" max="58" width="13.5703125" customWidth="1"/>
-    <col min="59" max="59" width="13" customWidth="1"/>
-    <col min="60" max="60" width="14" customWidth="1"/>
-    <col min="61" max="61" width="12.28515625" customWidth="1"/>
-    <col min="62" max="62" width="13.140625" customWidth="1"/>
-    <col min="75" max="85" width="9.140625" style="48"/>
+    <col min="57" max="57" width="29.7109375" customWidth="1"/>
+    <col min="58" max="58" width="18.85546875" customWidth="1"/>
+    <col min="59" max="59" width="19" customWidth="1"/>
+    <col min="60" max="60" width="29.85546875" customWidth="1"/>
+    <col min="61" max="61" width="22.140625" customWidth="1"/>
+    <col min="62" max="62" width="20.140625" customWidth="1"/>
+    <col min="63" max="63" width="32.85546875" customWidth="1"/>
+    <col min="64" max="64" width="21.28515625" customWidth="1"/>
+    <col min="65" max="65" width="19.42578125" customWidth="1"/>
+    <col min="66" max="66" width="22" customWidth="1"/>
+    <col min="67" max="67" width="19" customWidth="1"/>
+    <col min="68" max="68" width="18.28515625" customWidth="1"/>
+    <col min="69" max="69" width="43.85546875" customWidth="1"/>
+    <col min="70" max="70" width="41.85546875" customWidth="1"/>
+    <col min="71" max="71" width="23.140625" customWidth="1"/>
+    <col min="72" max="72" width="24.5703125" customWidth="1"/>
+    <col min="73" max="73" width="21" customWidth="1"/>
+    <col min="74" max="74" width="16.85546875" customWidth="1"/>
+    <col min="75" max="75" width="19.28515625" style="48" customWidth="1"/>
+    <col min="76" max="76" width="22.85546875" style="48" customWidth="1"/>
+    <col min="77" max="77" width="20" style="48" customWidth="1"/>
+    <col min="78" max="78" width="20.140625" style="48" customWidth="1"/>
+    <col min="79" max="79" width="21" style="48" customWidth="1"/>
+    <col min="80" max="80" width="22.42578125" style="48" customWidth="1"/>
+    <col min="81" max="81" width="18.5703125" style="48" customWidth="1"/>
+    <col min="82" max="82" width="21.42578125" style="48" customWidth="1"/>
+    <col min="83" max="83" width="23.28515625" style="48" customWidth="1"/>
+    <col min="84" max="84" width="18.7109375" style="48" customWidth="1"/>
+    <col min="85" max="85" width="21.85546875" style="48" customWidth="1"/>
+    <col min="86" max="86" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:86" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="52"/>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
-      <c r="AB1" s="52"/>
-      <c r="AC1" s="52"/>
-      <c r="AD1" s="52"/>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="52"/>
-      <c r="AG1" s="52"/>
-      <c r="AH1" s="52"/>
-      <c r="AI1" s="52"/>
-      <c r="AJ1" s="52"/>
-      <c r="AK1" s="52"/>
-      <c r="AL1" s="52"/>
-      <c r="AM1" s="52"/>
-      <c r="AN1" s="52"/>
-      <c r="AO1" s="52"/>
-      <c r="AP1" s="52"/>
-      <c r="AQ1" s="52"/>
-      <c r="AR1" s="52"/>
-      <c r="AS1" s="52"/>
-      <c r="AT1" s="52"/>
-      <c r="AU1" s="52"/>
-      <c r="AV1" s="52"/>
-      <c r="AW1" s="52"/>
-      <c r="AX1" s="52"/>
-      <c r="AY1" s="52"/>
-      <c r="AZ1" s="52"/>
-      <c r="BA1" s="52"/>
-      <c r="BB1" s="52"/>
-      <c r="BC1" s="52"/>
-      <c r="BD1" s="52"/>
-      <c r="BE1" s="52"/>
-      <c r="BF1" s="52"/>
-      <c r="BG1" s="52"/>
-      <c r="BH1" s="52"/>
-      <c r="BI1" s="52"/>
-      <c r="BJ1" s="52"/>
-      <c r="BK1" s="52"/>
-      <c r="BL1" s="52"/>
-      <c r="BM1" s="52"/>
-      <c r="BN1" s="52"/>
-      <c r="BO1" s="52"/>
-      <c r="BP1" s="52"/>
-      <c r="BQ1" s="52"/>
-      <c r="BR1" s="52"/>
-      <c r="BS1" s="52"/>
-      <c r="BT1" s="52"/>
-      <c r="BU1" s="52"/>
-      <c r="BV1" s="52"/>
-      <c r="BW1" s="52"/>
-      <c r="BX1" s="52"/>
-      <c r="BY1" s="52"/>
-      <c r="BZ1" s="52"/>
-      <c r="CA1" s="52"/>
-      <c r="CB1" s="52"/>
-      <c r="CC1" s="52"/>
-      <c r="CD1" s="52"/>
-      <c r="CE1" s="52"/>
-      <c r="CF1" s="52"/>
-    </row>
-    <row r="2" spans="1:85" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+      <c r="V1" s="56"/>
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="56"/>
+      <c r="AA1" s="56"/>
+      <c r="AB1" s="56"/>
+      <c r="AC1" s="56"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="56"/>
+      <c r="AG1" s="56"/>
+      <c r="AH1" s="56"/>
+      <c r="AI1" s="56"/>
+      <c r="AJ1" s="56"/>
+      <c r="AK1" s="56"/>
+      <c r="AL1" s="56"/>
+      <c r="AM1" s="56"/>
+      <c r="AN1" s="56"/>
+      <c r="AO1" s="56"/>
+      <c r="AP1" s="56"/>
+      <c r="AQ1" s="56"/>
+      <c r="AR1" s="56"/>
+      <c r="AS1" s="56"/>
+      <c r="AT1" s="56"/>
+      <c r="AU1" s="56"/>
+      <c r="AV1" s="56"/>
+      <c r="AW1" s="56"/>
+      <c r="AX1" s="56"/>
+      <c r="AY1" s="56"/>
+      <c r="AZ1" s="56"/>
+      <c r="BA1" s="56"/>
+      <c r="BB1" s="56"/>
+      <c r="BC1" s="56"/>
+      <c r="BD1" s="56"/>
+      <c r="BE1" s="56"/>
+      <c r="BF1" s="56"/>
+      <c r="BG1" s="56"/>
+      <c r="BH1" s="56"/>
+      <c r="BI1" s="56"/>
+      <c r="BJ1" s="56"/>
+      <c r="BK1" s="56"/>
+      <c r="BL1" s="56"/>
+      <c r="BM1" s="56"/>
+      <c r="BN1" s="56"/>
+      <c r="BO1" s="56"/>
+      <c r="BP1" s="56"/>
+      <c r="BQ1" s="56"/>
+      <c r="BR1" s="56"/>
+      <c r="BS1" s="56"/>
+      <c r="BT1" s="56"/>
+      <c r="BU1" s="56"/>
+      <c r="BV1" s="56"/>
+      <c r="BW1" s="56"/>
+      <c r="BX1" s="56"/>
+      <c r="BY1" s="56"/>
+      <c r="BZ1" s="56"/>
+      <c r="CA1" s="56"/>
+      <c r="CB1" s="56"/>
+      <c r="CC1" s="56"/>
+      <c r="CD1" s="56"/>
+      <c r="CE1" s="56"/>
+      <c r="CF1" s="56"/>
+    </row>
+    <row r="2" spans="1:86" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="A3" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
-      <c r="AC3" s="56"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="56"/>
-      <c r="AF3" s="56"/>
-      <c r="AG3" s="56"/>
-      <c r="AH3" s="56"/>
-      <c r="AI3" s="56"/>
-      <c r="AJ3" s="56"/>
-      <c r="AK3" s="56"/>
-      <c r="AL3" s="56"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="56"/>
-      <c r="AQ3" s="56"/>
-      <c r="AR3" s="56"/>
-      <c r="AS3" s="56"/>
-      <c r="AT3" s="56"/>
-      <c r="AU3" s="56"/>
-      <c r="AV3" s="56"/>
-      <c r="AW3" s="56"/>
-      <c r="AX3" s="56"/>
-      <c r="AY3" s="56"/>
-      <c r="AZ3" s="56"/>
-      <c r="BA3" s="56"/>
-      <c r="BB3" s="56"/>
-      <c r="BC3" s="56"/>
-      <c r="BD3" s="56"/>
-    </row>
-    <row r="4" spans="1:85" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AA3" s="60"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
+      <c r="AF3" s="60"/>
+      <c r="AG3" s="60"/>
+      <c r="AH3" s="60"/>
+      <c r="AI3" s="60"/>
+      <c r="AJ3" s="60"/>
+      <c r="AK3" s="60"/>
+      <c r="AL3" s="60"/>
+      <c r="AM3" s="60"/>
+      <c r="AN3" s="60"/>
+      <c r="AO3" s="60"/>
+      <c r="AP3" s="60"/>
+      <c r="AQ3" s="60"/>
+      <c r="AR3" s="60"/>
+      <c r="AS3" s="60"/>
+      <c r="AT3" s="60"/>
+      <c r="AU3" s="60"/>
+      <c r="AV3" s="60"/>
+      <c r="AW3" s="60"/>
+      <c r="AX3" s="60"/>
+      <c r="AY3" s="60"/>
+      <c r="AZ3" s="60"/>
+      <c r="BA3" s="60"/>
+      <c r="BB3" s="60"/>
+      <c r="BC3" s="60"/>
+      <c r="BD3" s="60"/>
+    </row>
+    <row r="4" spans="1:86" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="69">
+      <c r="B5" s="73">
         <v>42942.583333333336</v>
       </c>
-      <c r="C5" s="70"/>
+      <c r="C5" s="74"/>
       <c r="D5" s="42"/>
       <c r="E5" s="42"/>
       <c r="H5" s="39"/>
     </row>
-    <row r="6" spans="1:85" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:85" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="57" t="s">
+    <row r="6" spans="1:86" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:86" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="59"/>
-      <c r="Y7" s="60" t="s">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+      <c r="O7" s="62"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="62"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
-      <c r="AC7" s="61"/>
-      <c r="AD7" s="61"/>
-      <c r="AE7" s="61"/>
-      <c r="AF7" s="62"/>
-      <c r="AG7" s="63" t="s">
+      <c r="Z7" s="65"/>
+      <c r="AA7" s="65"/>
+      <c r="AB7" s="65"/>
+      <c r="AC7" s="65"/>
+      <c r="AD7" s="65"/>
+      <c r="AE7" s="65"/>
+      <c r="AF7" s="66"/>
+      <c r="AG7" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="AH7" s="64"/>
-      <c r="AI7" s="64"/>
-      <c r="AJ7" s="64"/>
-      <c r="AK7" s="64"/>
-      <c r="AL7" s="64"/>
-      <c r="AM7" s="64"/>
-      <c r="AN7" s="64"/>
-      <c r="AO7" s="65"/>
-      <c r="AP7" s="66" t="s">
+      <c r="AH7" s="68"/>
+      <c r="AI7" s="68"/>
+      <c r="AJ7" s="68"/>
+      <c r="AK7" s="68"/>
+      <c r="AL7" s="68"/>
+      <c r="AM7" s="68"/>
+      <c r="AN7" s="68"/>
+      <c r="AO7" s="69"/>
+      <c r="AP7" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="AQ7" s="67"/>
-      <c r="AR7" s="67"/>
-      <c r="AS7" s="67"/>
-      <c r="AT7" s="67"/>
-      <c r="AU7" s="67"/>
-      <c r="AV7" s="67"/>
-      <c r="AW7" s="68"/>
-      <c r="AX7" s="57" t="s">
+      <c r="AQ7" s="71"/>
+      <c r="AR7" s="71"/>
+      <c r="AS7" s="71"/>
+      <c r="AT7" s="71"/>
+      <c r="AU7" s="71"/>
+      <c r="AV7" s="71"/>
+      <c r="AW7" s="72"/>
+      <c r="AX7" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="AY7" s="58"/>
-      <c r="AZ7" s="58"/>
-      <c r="BA7" s="58"/>
-      <c r="BB7" s="58"/>
-      <c r="BC7" s="58"/>
-      <c r="BD7" s="58"/>
-      <c r="BE7" s="53" t="s">
+      <c r="AY7" s="62"/>
+      <c r="AZ7" s="62"/>
+      <c r="BA7" s="62"/>
+      <c r="BB7" s="62"/>
+      <c r="BC7" s="62"/>
+      <c r="BD7" s="62"/>
+      <c r="BE7" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="BF7" s="54"/>
-      <c r="BG7" s="54"/>
-      <c r="BH7" s="54"/>
-      <c r="BI7" s="54"/>
-      <c r="BJ7" s="55"/>
-      <c r="BK7" s="71" t="s">
+      <c r="BF7" s="58"/>
+      <c r="BG7" s="58"/>
+      <c r="BH7" s="58"/>
+      <c r="BI7" s="58"/>
+      <c r="BJ7" s="59"/>
+      <c r="BK7" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="BL7" s="72"/>
-      <c r="BM7" s="72"/>
-      <c r="BN7" s="72"/>
-      <c r="BO7" s="72"/>
-      <c r="BP7" s="72"/>
-      <c r="BQ7" s="72"/>
-      <c r="BR7" s="72"/>
-      <c r="BS7" s="72"/>
-      <c r="BT7" s="72"/>
-      <c r="BU7" s="72"/>
-      <c r="BV7" s="72"/>
-      <c r="BW7" s="72"/>
-      <c r="BX7" s="72"/>
-      <c r="BY7" s="72"/>
-      <c r="BZ7" s="72"/>
-      <c r="CA7" s="72"/>
-      <c r="CB7" s="72"/>
-      <c r="CC7" s="72"/>
-      <c r="CD7" s="72"/>
-      <c r="CE7" s="72"/>
-      <c r="CF7" s="72"/>
-      <c r="CG7" s="72"/>
-    </row>
-    <row r="8" spans="1:85" s="2" customFormat="1" ht="57.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BL7" s="54"/>
+      <c r="BM7" s="54"/>
+      <c r="BN7" s="54"/>
+      <c r="BO7" s="54"/>
+      <c r="BP7" s="54"/>
+      <c r="BQ7" s="54"/>
+      <c r="BR7" s="54"/>
+      <c r="BS7" s="54"/>
+      <c r="BT7" s="54"/>
+      <c r="BU7" s="54"/>
+      <c r="BV7" s="54"/>
+      <c r="BW7" s="54"/>
+      <c r="BX7" s="54"/>
+      <c r="BY7" s="54"/>
+      <c r="BZ7" s="54"/>
+      <c r="CA7" s="54"/>
+      <c r="CB7" s="54"/>
+      <c r="CC7" s="54"/>
+      <c r="CD7" s="54"/>
+      <c r="CE7" s="54"/>
+      <c r="CF7" s="54"/>
+      <c r="CG7" s="54"/>
+      <c r="CH7" s="54"/>
+    </row>
+    <row r="8" spans="1:86" s="2" customFormat="1" ht="57.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>3</v>
       </c>
@@ -1832,8 +1888,11 @@
       <c r="CG8" s="49" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="9" spans="1:85" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="CH8" s="52" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:86" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>26</v>
       </c>
@@ -1995,9 +2054,11 @@
       <c r="CE9" s="50"/>
       <c r="CF9" s="50"/>
       <c r="CG9" s="50"/>
+      <c r="CH9" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="BK7:CH7"/>
     <mergeCell ref="A1:CF1"/>
     <mergeCell ref="BE7:BJ7"/>
     <mergeCell ref="A3:BD3"/>
@@ -2007,7 +2068,6 @@
     <mergeCell ref="AP7:AW7"/>
     <mergeCell ref="AX7:BD7"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="BK7:CG7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -2018,197 +2078,200 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.42578125" customWidth="1"/>
-    <col min="5" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="38" width="15.42578125" customWidth="1"/>
-    <col min="39" max="39" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" customWidth="1"/>
+    <col min="12" max="12" width="46.5703125" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="20" width="15.42578125" customWidth="1"/>
+    <col min="21" max="21" width="23.42578125" customWidth="1"/>
+    <col min="22" max="38" width="15.42578125" customWidth="1"/>
+    <col min="39" max="39" width="27" customWidth="1"/>
     <col min="40" max="40" width="47.140625" customWidth="1"/>
-    <col min="41" max="41" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="31.42578125" customWidth="1"/>
-    <col min="43" max="43" width="12.7109375" customWidth="1"/>
-    <col min="44" max="44" width="28" customWidth="1"/>
+    <col min="41" max="41" width="19.5703125" customWidth="1"/>
+    <col min="42" max="42" width="39" customWidth="1"/>
+    <col min="43" max="43" width="29.7109375" customWidth="1"/>
+    <col min="44" max="44" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
-      <c r="AA1" s="74"/>
-      <c r="AB1" s="74"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="74"/>
-      <c r="AF1" s="74"/>
-      <c r="AG1" s="74"/>
-      <c r="AH1" s="74"/>
-      <c r="AI1" s="74"/>
-      <c r="AJ1" s="74"/>
-      <c r="AK1" s="74"/>
-      <c r="AL1" s="74"/>
-      <c r="AM1" s="74"/>
-      <c r="AN1" s="74"/>
-      <c r="AO1" s="74"/>
-      <c r="AP1" s="74"/>
-      <c r="AQ1" s="74"/>
-      <c r="AR1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="76"/>
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="76"/>
+      <c r="AH1" s="76"/>
+      <c r="AI1" s="76"/>
+      <c r="AJ1" s="76"/>
+      <c r="AK1" s="76"/>
+      <c r="AL1" s="76"/>
+      <c r="AM1" s="76"/>
+      <c r="AN1" s="76"/>
+      <c r="AO1" s="76"/>
+      <c r="AP1" s="76"/>
+      <c r="AQ1" s="76"/>
+      <c r="AR1" s="77"/>
     </row>
     <row r="2" spans="1:44" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="56"/>
-      <c r="S3" s="56"/>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
-      <c r="Z3" s="56"/>
-      <c r="AA3" s="56"/>
-      <c r="AB3" s="56"/>
-      <c r="AC3" s="56"/>
-      <c r="AD3" s="56"/>
-      <c r="AE3" s="56"/>
-      <c r="AF3" s="56"/>
-      <c r="AG3" s="56"/>
-      <c r="AH3" s="56"/>
-      <c r="AI3" s="56"/>
-      <c r="AJ3" s="56"/>
-      <c r="AK3" s="56"/>
-      <c r="AL3" s="56"/>
-      <c r="AM3" s="56"/>
-      <c r="AN3" s="56"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="56"/>
-      <c r="AQ3" s="56"/>
-      <c r="AR3" s="56"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="60"/>
+      <c r="T3" s="60"/>
+      <c r="U3" s="60"/>
+      <c r="V3" s="60"/>
+      <c r="W3" s="60"/>
+      <c r="X3" s="60"/>
+      <c r="Y3" s="60"/>
+      <c r="Z3" s="60"/>
+      <c r="AA3" s="60"/>
+      <c r="AB3" s="60"/>
+      <c r="AC3" s="60"/>
+      <c r="AD3" s="60"/>
+      <c r="AE3" s="60"/>
+      <c r="AF3" s="60"/>
+      <c r="AG3" s="60"/>
+      <c r="AH3" s="60"/>
+      <c r="AI3" s="60"/>
+      <c r="AJ3" s="60"/>
+      <c r="AK3" s="60"/>
+      <c r="AL3" s="60"/>
+      <c r="AM3" s="60"/>
+      <c r="AN3" s="60"/>
+      <c r="AO3" s="60"/>
+      <c r="AP3" s="60"/>
+      <c r="AQ3" s="60"/>
+      <c r="AR3" s="60"/>
     </row>
     <row r="4" spans="1:44" ht="6.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="69">
+      <c r="B5" s="73">
         <v>42942.583333333336</v>
       </c>
-      <c r="C5" s="69"/>
+      <c r="C5" s="73"/>
     </row>
     <row r="6" spans="1:44" ht="6.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:44" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="60" t="s">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="61"/>
-      <c r="R7" s="61"/>
-      <c r="S7" s="61"/>
-      <c r="T7" s="61"/>
-      <c r="U7" s="62"/>
-      <c r="V7" s="63" t="s">
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="65"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="66"/>
+      <c r="V7" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-      <c r="AC7" s="64"/>
-      <c r="AD7" s="65"/>
-      <c r="AE7" s="66" t="s">
+      <c r="W7" s="68"/>
+      <c r="X7" s="68"/>
+      <c r="Y7" s="68"/>
+      <c r="Z7" s="68"/>
+      <c r="AA7" s="68"/>
+      <c r="AB7" s="68"/>
+      <c r="AC7" s="68"/>
+      <c r="AD7" s="69"/>
+      <c r="AE7" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="AF7" s="67"/>
-      <c r="AG7" s="67"/>
-      <c r="AH7" s="67"/>
-      <c r="AI7" s="67"/>
-      <c r="AJ7" s="67"/>
-      <c r="AK7" s="67"/>
-      <c r="AL7" s="68"/>
-      <c r="AM7" s="57" t="s">
+      <c r="AF7" s="71"/>
+      <c r="AG7" s="71"/>
+      <c r="AH7" s="71"/>
+      <c r="AI7" s="71"/>
+      <c r="AJ7" s="71"/>
+      <c r="AK7" s="71"/>
+      <c r="AL7" s="72"/>
+      <c r="AM7" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="58"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="59"/>
+      <c r="AN7" s="62"/>
+      <c r="AO7" s="62"/>
+      <c r="AP7" s="62"/>
+      <c r="AQ7" s="62"/>
+      <c r="AR7" s="63"/>
     </row>
     <row r="8" spans="1:44" s="2" customFormat="1" ht="57.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">

</xml_diff>

<commit_message>
Updated Call Monitoring Report Template
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA939C5-8B0C-433D-8E54-C7A671FDD7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE934E7-448E-43B2-AE8C-B44E785DECF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CallMonitoringReport" sheetId="4" r:id="rId1"/>
@@ -329,8 +329,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -765,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -815,7 +815,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -845,7 +845,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -871,11 +871,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="5" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="5" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1296,14 +1296,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC331D33-4154-4CDD-B7F8-E59F04140001}">
   <dimension ref="A1:CH9"/>
   <sheetViews>
-    <sheetView topLeftCell="BP1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="BQ8" sqref="BQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
@@ -2078,7 +2078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Call Monitoring stats report update
</commit_message>
<xml_diff>
--- a/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
+++ b/UDM.Insurance.Interface/Templates/ReportTemplateCallMonitoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MbuleloD\source\repos\Insure\UDM.Insurance.Interface\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE934E7-448E-43B2-AE8C-B44E785DECF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA939C5-8B0C-433D-8E54-C7A671FDD7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CallMonitoringReport" sheetId="4" r:id="rId1"/>
@@ -329,8 +329,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="8" formatCode="&quot;R&quot;\ #,##0.00;[Red]&quot;R&quot;\ \-#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_ &quot;R&quot;\ * #,##0.00_ ;_ &quot;R&quot;\ * \-#,##0.00_ ;_ &quot;R&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -765,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -815,7 +815,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -845,7 +845,7 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -871,11 +871,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="5" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="5" fillId="13" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1296,14 +1296,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC331D33-4154-4CDD-B7F8-E59F04140001}">
   <dimension ref="A1:CH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="BP1" workbookViewId="0">
       <selection activeCell="BQ8" sqref="BQ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
@@ -2078,7 +2078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR9"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>